<commit_message>
Updated EDA correlation feature selection
Updated EDA correlation feature selection
</commit_message>
<xml_diff>
--- a/na_dropped_attributes.xlsx
+++ b/na_dropped_attributes.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mryua\MADS-CAPSTONE\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2485FDF7-9D4A-4B6E-B3BF-81453E132EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="na_rate_threshold-0.5" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -445,8 +439,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,25 +499,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -561,7 +547,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -595,7 +581,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -630,10 +615,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -806,20 +790,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="109" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -827,7 +805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -835,7 +813,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -843,7 +821,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -851,7 +829,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -859,7 +837,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -867,7 +845,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -875,7 +853,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -883,7 +861,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -891,7 +869,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -899,7 +877,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -907,7 +885,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -915,7 +893,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -923,7 +901,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -931,7 +909,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -939,7 +917,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -947,7 +925,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -955,7 +933,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -963,7 +941,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -971,7 +949,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -979,7 +957,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -987,7 +965,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -995,7 +973,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1003,7 +981,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1011,7 +989,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1019,7 +997,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1027,7 +1005,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1035,7 +1013,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1043,7 +1021,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1051,7 +1029,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1059,7 +1037,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1067,7 +1045,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1075,7 +1053,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1083,7 +1061,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1091,7 +1069,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1099,7 +1077,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1107,7 +1085,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1115,7 +1093,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1123,7 +1101,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1131,7 +1109,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1139,7 +1117,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1147,7 +1125,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1155,7 +1133,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -1163,7 +1141,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1171,7 +1149,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -1179,7 +1157,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -1187,7 +1165,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1195,7 +1173,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1203,7 +1181,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1211,7 +1189,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -1219,7 +1197,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -1227,7 +1205,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -1235,7 +1213,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -1243,7 +1221,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -1251,7 +1229,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -1259,7 +1237,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -1267,7 +1245,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -1275,7 +1253,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -1283,7 +1261,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -1291,7 +1269,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -1299,7 +1277,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -1307,7 +1285,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -1315,7 +1293,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -1323,7 +1301,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -1331,7 +1309,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -1339,7 +1317,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -1347,7 +1325,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -1355,7 +1333,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -1363,7 +1341,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -1371,7 +1349,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2">
       <c r="A70" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
Added dev/validation split, added lasso regression for feature selection
Lasso results need to be verified before proceeding
</commit_message>
<xml_diff>
--- a/na_dropped_attributes.xlsx
+++ b/na_dropped_attributes.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="na_rate_threshold-0.5" sheetId="1" r:id="rId1"/>
+    <sheet name="na_rate_threshold-0.2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="308">
   <si>
     <t>original_cname</t>
   </si>
@@ -22,6 +22,21 @@
     <t>mapped_cname</t>
   </si>
   <si>
+    <t>AMS3012</t>
+  </si>
+  <si>
+    <t>AMS3014</t>
+  </si>
+  <si>
+    <t>AMS3017</t>
+  </si>
+  <si>
+    <t>AMS3019</t>
+  </si>
+  <si>
+    <t>AMS3022</t>
+  </si>
+  <si>
     <t>AMS3025</t>
   </si>
   <si>
@@ -40,36 +55,69 @@
     <t>AMS3117</t>
   </si>
   <si>
+    <t>AMS3123</t>
+  </si>
+  <si>
+    <t>AMS3126</t>
+  </si>
+  <si>
     <t>AMS3132</t>
   </si>
   <si>
+    <t>AMS3138</t>
+  </si>
+  <si>
     <t>AMS3140</t>
   </si>
   <si>
+    <t>AMS3141</t>
+  </si>
+  <si>
     <t>AMS3143</t>
   </si>
   <si>
+    <t>AMS3144</t>
+  </si>
+  <si>
     <t>AMS3147</t>
   </si>
   <si>
     <t>AMS3152</t>
   </si>
   <si>
+    <t>AMS3158</t>
+  </si>
+  <si>
+    <t>AMS3160</t>
+  </si>
+  <si>
     <t>AMS3162</t>
   </si>
   <si>
     <t>AMS3163</t>
   </si>
   <si>
+    <t>AMS3164</t>
+  </si>
+  <si>
     <t>AMS3165</t>
   </si>
   <si>
+    <t>AMS3166</t>
+  </si>
+  <si>
+    <t>AMS3167</t>
+  </si>
+  <si>
     <t>AMS3169</t>
   </si>
   <si>
     <t>AMS3174</t>
   </si>
   <si>
+    <t>AMS3181</t>
+  </si>
+  <si>
     <t>AMS3183</t>
   </si>
   <si>
@@ -97,57 +145,198 @@
     <t>AMS3202</t>
   </si>
   <si>
+    <t>AMS3203</t>
+  </si>
+  <si>
     <t>AMS3205</t>
   </si>
   <si>
+    <t>AMS3206</t>
+  </si>
+  <si>
     <t>AMS3207</t>
   </si>
   <si>
+    <t>AMS3219</t>
+  </si>
+  <si>
+    <t>AMS3220</t>
+  </si>
+  <si>
+    <t>AMS3234</t>
+  </si>
+  <si>
+    <t>AMS3272</t>
+  </si>
+  <si>
+    <t>AMS3292</t>
+  </si>
+  <si>
+    <t>AMS3311</t>
+  </si>
+  <si>
+    <t>AMS3322</t>
+  </si>
+  <si>
+    <t>AMS3332</t>
+  </si>
+  <si>
+    <t>AMS3351</t>
+  </si>
+  <si>
+    <t>AMS3357</t>
+  </si>
+  <si>
+    <t>AMS3363</t>
+  </si>
+  <si>
+    <t>AMS3371</t>
+  </si>
+  <si>
+    <t>AMS3382</t>
+  </si>
+  <si>
     <t>AMS3387</t>
   </si>
   <si>
+    <t>AMS3391</t>
+  </si>
+  <si>
     <t>AMS3396</t>
   </si>
   <si>
+    <t>AMS3400</t>
+  </si>
+  <si>
     <t>AMS3405</t>
   </si>
   <si>
+    <t>AMS3409</t>
+  </si>
+  <si>
     <t>AMS3414</t>
   </si>
   <si>
+    <t>AMS3419</t>
+  </si>
+  <si>
+    <t>AMS3422</t>
+  </si>
+  <si>
     <t>AMS3425</t>
   </si>
   <si>
+    <t>AMS3430</t>
+  </si>
+  <si>
+    <t>AMS3433</t>
+  </si>
+  <si>
     <t>AMS3436</t>
   </si>
   <si>
+    <t>AMS3441</t>
+  </si>
+  <si>
+    <t>AMS3444</t>
+  </si>
+  <si>
     <t>AMS3447</t>
   </si>
   <si>
+    <t>AMS3452</t>
+  </si>
+  <si>
+    <t>AMS3455</t>
+  </si>
+  <si>
     <t>AMS3458</t>
   </si>
   <si>
+    <t>AMS3536</t>
+  </si>
+  <si>
+    <t>AMS3539</t>
+  </si>
+  <si>
+    <t>AMS3547</t>
+  </si>
+  <si>
+    <t>AMS3550</t>
+  </si>
+  <si>
+    <t>AMS3558</t>
+  </si>
+  <si>
+    <t>AMS3561</t>
+  </si>
+  <si>
+    <t>AMS3569</t>
+  </si>
+  <si>
+    <t>AMS3572</t>
+  </si>
+  <si>
+    <t>AMS3579</t>
+  </si>
+  <si>
     <t>AMS3580</t>
   </si>
   <si>
+    <t>AMS3585</t>
+  </si>
+  <si>
+    <t>AMS3593</t>
+  </si>
+  <si>
+    <t>AMS3596</t>
+  </si>
+  <si>
     <t>AMS3598</t>
   </si>
   <si>
     <t>AMS3602</t>
   </si>
   <si>
+    <t>AMS3607</t>
+  </si>
+  <si>
+    <t>AMS3609</t>
+  </si>
+  <si>
     <t>AMS3610</t>
   </si>
   <si>
+    <t>AMS3618</t>
+  </si>
+  <si>
     <t>AMS3624</t>
   </si>
   <si>
+    <t>AMS3629</t>
+  </si>
+  <si>
+    <t>AMS3723</t>
+  </si>
+  <si>
+    <t>AMS3725</t>
+  </si>
+  <si>
     <t>AMS3727</t>
   </si>
   <si>
+    <t>AMS3728</t>
+  </si>
+  <si>
     <t>AMS3729</t>
   </si>
   <si>
+    <t>AMS3749</t>
+  </si>
+  <si>
+    <t>AMS3759</t>
+  </si>
+  <si>
     <t>AMS3760</t>
   </si>
   <si>
@@ -190,6 +379,9 @@
     <t>AMS3808</t>
   </si>
   <si>
+    <t>AMS3809</t>
+  </si>
+  <si>
     <t>AMS3812</t>
   </si>
   <si>
@@ -202,24 +394,57 @@
     <t>AMS3815</t>
   </si>
   <si>
+    <t>AMS3830</t>
+  </si>
+  <si>
+    <t>AMS3834</t>
+  </si>
+  <si>
     <t>AMS3848</t>
   </si>
   <si>
     <t>AMS3849</t>
   </si>
   <si>
+    <t>AMS3850</t>
+  </si>
+  <si>
+    <t>AMS3851</t>
+  </si>
+  <si>
     <t>AMS3853</t>
   </si>
   <si>
     <t>AMS3855</t>
   </si>
   <si>
+    <t>AMS3857</t>
+  </si>
+  <si>
+    <t>AMS3858</t>
+  </si>
+  <si>
     <t>AMS3859</t>
   </si>
   <si>
+    <t>AMS3861</t>
+  </si>
+  <si>
     <t>AMS3867</t>
   </si>
   <si>
+    <t>AMS3876</t>
+  </si>
+  <si>
+    <t>AMS3877</t>
+  </si>
+  <si>
+    <t>AMS3878</t>
+  </si>
+  <si>
+    <t>AMS3890</t>
+  </si>
+  <si>
     <t>AMS3911</t>
   </si>
   <si>
@@ -229,6 +454,48 @@
     <t>AMS3913</t>
   </si>
   <si>
+    <t>AMS3923</t>
+  </si>
+  <si>
+    <t>AMS3924</t>
+  </si>
+  <si>
+    <t>AMS3925</t>
+  </si>
+  <si>
+    <t>AMS3956</t>
+  </si>
+  <si>
+    <t>AMS3957</t>
+  </si>
+  <si>
+    <t>AMS3958</t>
+  </si>
+  <si>
+    <t>AMS3985</t>
+  </si>
+  <si>
+    <t>AMS3990</t>
+  </si>
+  <si>
+    <t>AMS3993</t>
+  </si>
+  <si>
+    <t>% Inq w/in 1 Month to Inq w/in 12 M</t>
+  </si>
+  <si>
+    <t>% Util Inq w/in 3 M to Inq w/in 12 M</t>
+  </si>
+  <si>
+    <t>% Util Inq w/in 1 Month to Inq w/in 12 M</t>
+  </si>
+  <si>
+    <t>% Non-Util Inq w/in 3 M to Inq w/in 12 M</t>
+  </si>
+  <si>
+    <t>% Non-Util Inq w/in 1 Month to Inq w/in 12 M</t>
+  </si>
+  <si>
     <t># Util Inq w/in 6 M</t>
   </si>
   <si>
@@ -247,36 +514,69 @@
     <t>Age Oldest Mortgage Trade</t>
   </si>
   <si>
+    <t>Age Newest Auto Trade</t>
+  </si>
+  <si>
+    <t>Age Newest Dept Store Trades</t>
+  </si>
+  <si>
     <t>Age Newest Sales Finance Trade</t>
   </si>
   <si>
+    <t># Open Auto Trades</t>
+  </si>
+  <si>
     <t># Open Credit Union Trades</t>
   </si>
   <si>
+    <t># Open Dept Store Trades</t>
+  </si>
+  <si>
     <t># Open Mortgage Trades</t>
   </si>
   <si>
+    <t># Open PerFin and StuLoan Trades</t>
+  </si>
+  <si>
     <t># Open Sales Finance Trades</t>
   </si>
   <si>
     <t xml:space="preserve"># Dept Store Trades w/Update w/in 3 M w/ Bal &gt; $0 </t>
   </si>
   <si>
+    <t xml:space="preserve"># Retail Trades w/Update w/in 3 M w/ Bal &gt; $0 </t>
+  </si>
+  <si>
+    <t>T Bal Open Auto Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
     <t>T Bal Open Credit Union Trades w/Update w/in 3 M</t>
   </si>
   <si>
     <t>T Bal Open Dept Store Trades w/Update w/in 3 M</t>
   </si>
   <si>
+    <t>T Bal Open Inst Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
     <t>T Bal Open Mortgage Trades w/Update w/in 3 M</t>
   </si>
   <si>
+    <t>T Bal Open PerFin and StuLoan Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
+    <t>T Bal Open Retail Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
     <t>T Bal Open Sales Finance Trades w/Update w/in 3 M</t>
   </si>
   <si>
     <t>T Bal Open StuLoan Trades w/Update w/in 3 M</t>
   </si>
   <si>
+    <t>T Bal Closed Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
     <t>T Bal Closed Bkcrd Trades w/Update w/in 3 M</t>
   </si>
   <si>
@@ -304,57 +604,198 @@
     <t>T Loan Amount Open StuLoan Trades w/Update w/in 3 M</t>
   </si>
   <si>
+    <t>T Loan Amount Open Auto Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
     <t>T High Credit Open Dept Store Trades w/Update w/in 3 M</t>
   </si>
   <si>
+    <t>T Loan Amount Open Inst Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
     <t>T Loan Amount Open Mortgage Trades w/Update w/in 3 M</t>
   </si>
   <si>
+    <t># Dept Store Trades w/ PD &gt; $0</t>
+  </si>
+  <si>
+    <t>T High Credit Open Retail Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
+    <t>T PD Retail Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
+    <t># 30 DPD Occur w/in 24 M Dept Store Trades</t>
+  </si>
+  <si>
+    <t># 60 DPD Occur w/in 24 M Dept Store Trades</t>
+  </si>
+  <si>
+    <t># 90 DPD Occur w/in 24 M Dept Store Trades</t>
+  </si>
+  <si>
+    <t># 120-180 or More DPD Occur w/in 24 M Dept Store Trades</t>
+  </si>
+  <si>
+    <t># Dept Store Trades Satis w/in 3 M</t>
+  </si>
+  <si>
+    <t># 60-180 or More DPD Occur w/in 24 M Dept Store Trades</t>
+  </si>
+  <si>
+    <t># 90-180 or More DPD Occur w/in 24 M Dept Store Trades</t>
+  </si>
+  <si>
+    <t># 60-180 or More DPD Occur w/in 12 M Dept Store Trades</t>
+  </si>
+  <si>
+    <t># 90-180 or More DPD Occur w/in 12 M Dept Store Trades</t>
+  </si>
+  <si>
+    <t># Dept Store Tr Wo Rat 30 DPD w/in 3 M</t>
+  </si>
+  <si>
     <t># Sales Finance Tr Wo Rat 30 DPD w/in 3 M</t>
   </si>
   <si>
+    <t># Dept Store Tr Wo Rat 60 DPD w/in 3 M</t>
+  </si>
+  <si>
     <t># Sales Finance Tr Wo Rat 60 DPD w/in 3 M</t>
   </si>
   <si>
+    <t># Dept Store Tr Wo Rat 90 DPD w/in 3 M</t>
+  </si>
+  <si>
     <t># Sales Finance Tr Wo Rat 90 DPD w/in 3 M</t>
   </si>
   <si>
+    <t># Dept Store Tr Wo Rat 120-180 or More DPD w/in 3 M</t>
+  </si>
+  <si>
     <t># Sales Finance Tr Wo Rat 120-180 or More DPD w/in 3 M</t>
   </si>
   <si>
+    <t># Dept Store Tr Wo Rat 30 DPD w/in 6 M</t>
+  </si>
+  <si>
+    <t># PerFin and StuLoan Tr Wo Rat 30 DPD w/in 6 M</t>
+  </si>
+  <si>
     <t># Sales Finance Tr Wo Rat 30 DPD w/in 6 M</t>
   </si>
   <si>
+    <t># Dept Store Tr Wo Rat 60 DPD w/in 6 M</t>
+  </si>
+  <si>
+    <t># PerFin and StuLoan Tr Wo Rat 60 DPD w/in 6 M</t>
+  </si>
+  <si>
     <t># Sales Finance Tr Wo Rat 60 DPD w/in 6 M</t>
   </si>
   <si>
+    <t># Dept Store Tr Wo Rat 90 DPD w/in 6 M</t>
+  </si>
+  <si>
+    <t># PerFin and StuLoan Tr Wo Rat 90 DPD w/in 6 M</t>
+  </si>
+  <si>
     <t># Sales Finance Tr Wo Rat 90 DPD w/in 6 M</t>
   </si>
   <si>
+    <t># Dept Store Tr Wo Rat 120-180 or More DPD w/in 6 M</t>
+  </si>
+  <si>
+    <t># PerFin and StuLoan Tr Wo Rat 120-180 or More DPD w/in 6 M</t>
+  </si>
+  <si>
     <t># Sales Finance Tr Wo Rat 120-180 or More DPD w/in 6 M</t>
   </si>
   <si>
+    <t># Auto Tr Wo Rat Ever 30 DPD</t>
+  </si>
+  <si>
+    <t># Dept Store Tr Wo Rat Ever 30 DPD</t>
+  </si>
+  <si>
+    <t># Auto Tr Wo Rat Ever 60 DPD</t>
+  </si>
+  <si>
+    <t># Dept Store Tr Wo Rat Ever 60 DPD</t>
+  </si>
+  <si>
+    <t># Auto Tr Wo Rat Ever 90 DPD</t>
+  </si>
+  <si>
+    <t># Dept Store Tr Wo Rat Ever 90 DPD</t>
+  </si>
+  <si>
+    <t># Auto Tr Wo Rat Ever 120-180 or More DPD</t>
+  </si>
+  <si>
+    <t># Dept Store Tr Wo Rat Ever 120-180 or More DPD</t>
+  </si>
+  <si>
+    <t>Worst Rating w/in 3 M Auto Trades</t>
+  </si>
+  <si>
     <t>Worst Rating w/in 3 M Mortgage Trades</t>
   </si>
   <si>
+    <t># Dept Store Trades w/ MajDerog Reported w/in 6 M</t>
+  </si>
+  <si>
+    <t># Auto Trades w/ MajDerog Event w/in 24 M</t>
+  </si>
+  <si>
+    <t># Dept Store Trades w/ MajDerog Event w/in 24 M</t>
+  </si>
+  <si>
     <t># Mortgage Trades w/ MajDerog Event w/in 24 M</t>
   </si>
   <si>
     <t># Sales Finance Trades w/ MajDerog Event w/in 24 M</t>
   </si>
   <si>
+    <t># Dept Store Trades MajDerog</t>
+  </si>
+  <si>
+    <t># Auto Trades MajDerog</t>
+  </si>
+  <si>
     <t># Mortgage Trades MajDerog</t>
   </si>
   <si>
+    <t># Dept Store Trades w/ Unpaid MajDerog Event w/in 24 M</t>
+  </si>
+  <si>
     <t># Sales Finance Trades w/ Unpaid MajDerog Event w/in 24 M</t>
   </si>
   <si>
+    <t xml:space="preserve"># Dept Store Trades Unpaid MajDerog </t>
+  </si>
+  <si>
+    <t># Open Retail Trades w/ Update w/in 3 M w/ Bal &gt;= 50% High Credit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Open Auto Trades w/ Update w/in 3 M w/ Bal &gt;= 75% Loan Amount </t>
+  </si>
+  <si>
     <t xml:space="preserve"># Open Dept Store Trades w/ Update w/in 3 M w/ Bal &gt;= 75% High Credit </t>
   </si>
   <si>
+    <t xml:space="preserve"># Open Inst Trades w/ Update w/in 3 M w/ Bal &gt;= 75% Loan Amount </t>
+  </si>
+  <si>
     <t xml:space="preserve"># Open Mortgage Trades w/ Update w/in 3 M w/ Bal &gt;= 75% Loan Amount </t>
   </si>
   <si>
+    <t># Dept Store Trades Reported w/in 3 M</t>
+  </si>
+  <si>
+    <t>Age Newest Date Last Activity Trades Other Than Paid as Agreed</t>
+  </si>
+  <si>
     <t>Age Newest Date Last Activity Bkcrd Trades Other Than Paid as Agreed</t>
   </si>
   <si>
@@ -397,6 +838,9 @@
     <t>T Bal Defaulted StuLoan Trades w/Update w/in 3 M</t>
   </si>
   <si>
+    <t>% Bal to High Credit Open Retail Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
     <t>Age Newest Tax Lien Public Record Item</t>
   </si>
   <si>
@@ -409,24 +853,57 @@
     <t># of Judgment Pub Rec Item</t>
   </si>
   <si>
+    <t>% Open Dept Store Trades to Open Retail Trades</t>
+  </si>
+  <si>
+    <t>% Open Dept Store Trades to Dept Store Trades</t>
+  </si>
+  <si>
     <t>T Bal Credit Union Trades w/Update w/in 3 M</t>
   </si>
   <si>
     <t>T Bal Dept Store Trades w/Update w/in 3 M</t>
   </si>
   <si>
+    <t>T Bal PerFin and StuLoan Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
+    <t>T Bal Retail Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
     <t>T Bal Sales Finance Trades w/Update w/in 3 M</t>
   </si>
   <si>
     <t>% Bal to High Credit Open Dept Store Trades w/Update w/in 3 M</t>
   </si>
   <si>
+    <t>% Bal to T Loan Amount Open Auto Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
+    <t>% Bal to T Loan Amount Open Inst Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
     <t>% Bal to T Loan Amount Open Mortgage Trades w/Update w/in 3 M</t>
   </si>
   <si>
+    <t>% T PD to T Bal Retail Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
     <t>% Dept Store Trades Satis w/in 3 M to Dept Store Trades Reported w/in 3 M</t>
   </si>
   <si>
+    <t># Dept Store Tr Wo Rat 60 DPD or Worse w/in 3 M or MajDerog Event w/in 24 M</t>
+  </si>
+  <si>
+    <t># Dept Store Tr Wo Rat 90 DPD or Worse w/in 3 M or MajDerog Event w/in 24 M</t>
+  </si>
+  <si>
+    <t># Dept Store Tr Wo Rat 120-180 or More DPD or Worse w/in 3 M or MajDerog Event w/in 24 M</t>
+  </si>
+  <si>
+    <t># Dept Store Tr Wo Rat No Worse Than 59 DPD w/in 3 M</t>
+  </si>
+  <si>
     <t>T Collection Amount 3rd Party Collections w/in 12 M</t>
   </si>
   <si>
@@ -434,6 +911,33 @@
   </si>
   <si>
     <t>T Collection Amount 3rd Party Collections</t>
+  </si>
+  <si>
+    <t># Dept Store Tr Wo Rat 60 DPD or Worse w/in 6 M or MajDerog Event w/in 24 M</t>
+  </si>
+  <si>
+    <t># Dept Store Tr Wo Rat 90 DPD or Worse w/in 6 M or MajDerog Event w/in 24 M</t>
+  </si>
+  <si>
+    <t># Dept Store Tr Wo Rat 120-180 or More DPD or Worse w/in 6 M or MajDerog Event w/in 24 M</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Dept Store Tr Wo Rat Ever 60 DPD or Worse </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Dept Store Tr Wo Rat Ever 90 DPD or Worse </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Dept Store Tr Wo Rat Ever 120-180 or More DPD or Worse </t>
+  </si>
+  <si>
+    <t>% Dept Store Trades w/MajDerog Event w/in 24 M to Dept Store Trades</t>
+  </si>
+  <si>
+    <t>% Dept Store Trades w/Unpaid MajDerog Event w/in 24 M to Dept Store Trades</t>
+  </si>
+  <si>
+    <t>% Inq w/in 3 M to Inq w/in 12 M</t>
   </si>
 </sst>
 </file>
@@ -791,7 +1295,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -810,7 +1314,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -818,7 +1322,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -826,7 +1330,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -834,7 +1338,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -842,7 +1346,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -850,7 +1354,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -858,7 +1362,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -866,7 +1370,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -874,7 +1378,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -882,7 +1386,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -890,7 +1394,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -898,7 +1402,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -906,7 +1410,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -914,7 +1418,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -922,7 +1426,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -930,7 +1434,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -938,7 +1442,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -946,7 +1450,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -954,7 +1458,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -962,7 +1466,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -970,7 +1474,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>91</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -978,7 +1482,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -986,7 +1490,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -994,7 +1498,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1002,7 +1506,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1010,7 +1514,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1018,7 +1522,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1026,7 +1530,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>98</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1034,7 +1538,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>99</v>
+        <v>183</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1042,7 +1546,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>184</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1050,7 +1554,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>101</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1058,7 +1562,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>102</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1066,7 +1570,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>187</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1074,7 +1578,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>104</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1082,7 +1586,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>105</v>
+        <v>189</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1090,7 +1594,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1098,7 +1602,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1106,7 +1610,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>108</v>
+        <v>192</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1114,7 +1618,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>109</v>
+        <v>193</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1122,7 +1626,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>110</v>
+        <v>194</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1130,7 +1634,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>111</v>
+        <v>195</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1138,7 +1642,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>196</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1146,7 +1650,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>113</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1154,7 +1658,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>114</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1162,7 +1666,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>115</v>
+        <v>199</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1170,7 +1674,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
+        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1178,7 +1682,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>201</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1186,7 +1690,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>118</v>
+        <v>202</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1194,7 +1698,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>119</v>
+        <v>203</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1202,7 +1706,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>120</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1210,7 +1714,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>121</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1218,7 +1722,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>122</v>
+        <v>206</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1226,7 +1730,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>123</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1234,7 +1738,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>124</v>
+        <v>208</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1242,7 +1746,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>125</v>
+        <v>209</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1250,7 +1754,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>126</v>
+        <v>210</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1258,7 +1762,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>127</v>
+        <v>211</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1266,7 +1770,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>128</v>
+        <v>212</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1274,7 +1778,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>129</v>
+        <v>213</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1282,7 +1786,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>130</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1290,7 +1794,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>131</v>
+        <v>215</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1298,7 +1802,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1306,7 +1810,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>133</v>
+        <v>217</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1314,7 +1818,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>134</v>
+        <v>218</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1322,7 +1826,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1330,7 +1834,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>136</v>
+        <v>220</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1338,7 +1842,7 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>137</v>
+        <v>221</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1346,7 +1850,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1354,7 +1858,679 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>73</v>
+      </c>
+      <c r="B73" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>74</v>
+      </c>
+      <c r="B74" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>76</v>
+      </c>
+      <c r="B76" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>77</v>
+      </c>
+      <c r="B77" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>78</v>
+      </c>
+      <c r="B78" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>80</v>
+      </c>
+      <c r="B80" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>82</v>
+      </c>
+      <c r="B82" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>83</v>
+      </c>
+      <c r="B83" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>87</v>
+      </c>
+      <c r="B87" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>88</v>
+      </c>
+      <c r="B88" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>89</v>
+      </c>
+      <c r="B89" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>90</v>
+      </c>
+      <c r="B90" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>91</v>
+      </c>
+      <c r="B91" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>92</v>
+      </c>
+      <c r="B92" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>93</v>
+      </c>
+      <c r="B93" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>94</v>
+      </c>
+      <c r="B94" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>95</v>
+      </c>
+      <c r="B95" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>96</v>
+      </c>
+      <c r="B96" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>97</v>
+      </c>
+      <c r="B97" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>98</v>
+      </c>
+      <c r="B98" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>99</v>
+      </c>
+      <c r="B99" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>100</v>
+      </c>
+      <c r="B100" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>101</v>
+      </c>
+      <c r="B101" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>102</v>
+      </c>
+      <c r="B102" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>103</v>
+      </c>
+      <c r="B103" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>104</v>
+      </c>
+      <c r="B104" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>105</v>
+      </c>
+      <c r="B105" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>106</v>
+      </c>
+      <c r="B106" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>107</v>
+      </c>
+      <c r="B107" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>108</v>
+      </c>
+      <c r="B108" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>109</v>
+      </c>
+      <c r="B109" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>110</v>
+      </c>
+      <c r="B110" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>111</v>
+      </c>
+      <c r="B111" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>112</v>
+      </c>
+      <c r="B112" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>113</v>
+      </c>
+      <c r="B113" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>114</v>
+      </c>
+      <c r="B114" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>115</v>
+      </c>
+      <c r="B115" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>116</v>
+      </c>
+      <c r="B116" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>117</v>
+      </c>
+      <c r="B117" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>118</v>
+      </c>
+      <c r="B118" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>119</v>
+      </c>
+      <c r="B119" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>120</v>
+      </c>
+      <c r="B120" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>121</v>
+      </c>
+      <c r="B121" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>122</v>
+      </c>
+      <c r="B122" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>123</v>
+      </c>
+      <c r="B123" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>124</v>
+      </c>
+      <c r="B124" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>125</v>
+      </c>
+      <c r="B125" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>126</v>
+      </c>
+      <c r="B126" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
+        <v>127</v>
+      </c>
+      <c r="B127" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>128</v>
+      </c>
+      <c r="B128" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" t="s">
+        <v>129</v>
+      </c>
+      <c r="B129" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" t="s">
+        <v>130</v>
+      </c>
+      <c r="B130" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" t="s">
+        <v>131</v>
+      </c>
+      <c r="B131" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" t="s">
+        <v>132</v>
+      </c>
+      <c r="B132" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" t="s">
+        <v>133</v>
+      </c>
+      <c r="B133" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" t="s">
+        <v>134</v>
+      </c>
+      <c r="B134" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" t="s">
+        <v>135</v>
+      </c>
+      <c r="B135" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" t="s">
+        <v>136</v>
+      </c>
+      <c r="B136" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" t="s">
+        <v>137</v>
+      </c>
+      <c r="B137" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" t="s">
+        <v>138</v>
+      </c>
+      <c r="B138" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" t="s">
         <v>139</v>
+      </c>
+      <c r="B139" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" t="s">
+        <v>140</v>
+      </c>
+      <c r="B140" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" t="s">
+        <v>141</v>
+      </c>
+      <c r="B141" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" t="s">
+        <v>142</v>
+      </c>
+      <c r="B142" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
+        <v>143</v>
+      </c>
+      <c r="B143" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" t="s">
+        <v>144</v>
+      </c>
+      <c r="B144" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" t="s">
+        <v>145</v>
+      </c>
+      <c r="B145" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" t="s">
+        <v>146</v>
+      </c>
+      <c r="B146" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" t="s">
+        <v>147</v>
+      </c>
+      <c r="B147" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" t="s">
+        <v>148</v>
+      </c>
+      <c r="B148" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" t="s">
+        <v>149</v>
+      </c>
+      <c r="B149" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" t="s">
+        <v>150</v>
+      </c>
+      <c r="B150" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
+        <v>151</v>
+      </c>
+      <c r="B151" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" t="s">
+        <v>152</v>
+      </c>
+      <c r="B152" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" t="s">
+        <v>153</v>
+      </c>
+      <c r="B153" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" t="s">
+        <v>154</v>
+      </c>
+      <c r="B154" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added random forest for feature selection. Added XGB and achieved 0.87 CV score
</commit_message>
<xml_diff>
--- a/na_dropped_attributes.xlsx
+++ b/na_dropped_attributes.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="na_rate_threshold-0.2" sheetId="1" r:id="rId1"/>
+    <sheet name="na_rate_threshold-0.1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="474">
   <si>
     <t>original_cname</t>
   </si>
@@ -22,24 +22,75 @@
     <t>mapped_cname</t>
   </si>
   <si>
+    <t>AMS3000</t>
+  </si>
+  <si>
+    <t>AMS3001</t>
+  </si>
+  <si>
+    <t>AMS3002</t>
+  </si>
+  <si>
+    <t>AMS3008</t>
+  </si>
+  <si>
+    <t>AMS3009</t>
+  </si>
+  <si>
+    <t>AMS3010</t>
+  </si>
+  <si>
+    <t>AMS3011</t>
+  </si>
+  <si>
     <t>AMS3012</t>
   </si>
   <si>
+    <t>AMS3013</t>
+  </si>
+  <si>
     <t>AMS3014</t>
   </si>
   <si>
+    <t>AMS3015</t>
+  </si>
+  <si>
+    <t>AMS3016</t>
+  </si>
+  <si>
     <t>AMS3017</t>
   </si>
   <si>
+    <t>AMS3018</t>
+  </si>
+  <si>
     <t>AMS3019</t>
   </si>
   <si>
+    <t>AMS3020</t>
+  </si>
+  <si>
+    <t>AMS3021</t>
+  </si>
+  <si>
     <t>AMS3022</t>
   </si>
   <si>
+    <t>AMS3023</t>
+  </si>
+  <si>
+    <t>AMS3024</t>
+  </si>
+  <si>
     <t>AMS3025</t>
   </si>
   <si>
+    <t>AMS3026</t>
+  </si>
+  <si>
+    <t>AMS3027</t>
+  </si>
+  <si>
     <t>AMS3028</t>
   </si>
   <si>
@@ -55,12 +106,18 @@
     <t>AMS3117</t>
   </si>
   <si>
+    <t>AMS3119</t>
+  </si>
+  <si>
     <t>AMS3123</t>
   </si>
   <si>
     <t>AMS3126</t>
   </si>
   <si>
+    <t>AMS3131</t>
+  </si>
+  <si>
     <t>AMS3132</t>
   </si>
   <si>
@@ -79,18 +136,30 @@
     <t>AMS3144</t>
   </si>
   <si>
+    <t>AMS3145</t>
+  </si>
+  <si>
     <t>AMS3147</t>
   </si>
   <si>
+    <t>AMS3150</t>
+  </si>
+  <si>
     <t>AMS3152</t>
   </si>
   <si>
+    <t>AMS3153</t>
+  </si>
+  <si>
     <t>AMS3158</t>
   </si>
   <si>
     <t>AMS3160</t>
   </si>
   <si>
+    <t>AMS3161</t>
+  </si>
+  <si>
     <t>AMS3162</t>
   </si>
   <si>
@@ -148,6 +217,9 @@
     <t>AMS3203</t>
   </si>
   <si>
+    <t>AMS3204</t>
+  </si>
+  <si>
     <t>AMS3205</t>
   </si>
   <si>
@@ -163,57 +235,117 @@
     <t>AMS3220</t>
   </si>
   <si>
+    <t>AMS3223</t>
+  </si>
+  <si>
+    <t>AMS3228</t>
+  </si>
+  <si>
+    <t>AMS3231</t>
+  </si>
+  <si>
     <t>AMS3234</t>
   </si>
   <si>
+    <t>AMS3245</t>
+  </si>
+  <si>
     <t>AMS3272</t>
   </si>
   <si>
+    <t>AMS3276</t>
+  </si>
+  <si>
+    <t>AMS3285</t>
+  </si>
+  <si>
     <t>AMS3292</t>
   </si>
   <si>
+    <t>AMS3296</t>
+  </si>
+  <si>
     <t>AMS3311</t>
   </si>
   <si>
+    <t>AMS3315</t>
+  </si>
+  <si>
     <t>AMS3322</t>
   </si>
   <si>
+    <t>AMS3326</t>
+  </si>
+  <si>
     <t>AMS3332</t>
   </si>
   <si>
+    <t>AMS3335</t>
+  </si>
+  <si>
+    <t>AMS3348</t>
+  </si>
+  <si>
     <t>AMS3351</t>
   </si>
   <si>
+    <t>AMS3353</t>
+  </si>
+  <si>
     <t>AMS3357</t>
   </si>
   <si>
+    <t>AMS3359</t>
+  </si>
+  <si>
     <t>AMS3363</t>
   </si>
   <si>
+    <t>AMS3365</t>
+  </si>
+  <si>
     <t>AMS3371</t>
   </si>
   <si>
+    <t>AMS3373</t>
+  </si>
+  <si>
+    <t>AMS3377</t>
+  </si>
+  <si>
     <t>AMS3382</t>
   </si>
   <si>
+    <t>AMS3385</t>
+  </si>
+  <si>
     <t>AMS3387</t>
   </si>
   <si>
     <t>AMS3391</t>
   </si>
   <si>
+    <t>AMS3394</t>
+  </si>
+  <si>
     <t>AMS3396</t>
   </si>
   <si>
     <t>AMS3400</t>
   </si>
   <si>
+    <t>AMS3403</t>
+  </si>
+  <si>
     <t>AMS3405</t>
   </si>
   <si>
     <t>AMS3409</t>
   </si>
   <si>
+    <t>AMS3412</t>
+  </si>
+  <si>
     <t>AMS3414</t>
   </si>
   <si>
@@ -223,6 +355,9 @@
     <t>AMS3422</t>
   </si>
   <si>
+    <t>AMS3423</t>
+  </si>
+  <si>
     <t>AMS3425</t>
   </si>
   <si>
@@ -232,6 +367,9 @@
     <t>AMS3433</t>
   </si>
   <si>
+    <t>AMS3434</t>
+  </si>
+  <si>
     <t>AMS3436</t>
   </si>
   <si>
@@ -241,6 +379,9 @@
     <t>AMS3444</t>
   </si>
   <si>
+    <t>AMS3445</t>
+  </si>
+  <si>
     <t>AMS3447</t>
   </si>
   <si>
@@ -250,6 +391,9 @@
     <t>AMS3455</t>
   </si>
   <si>
+    <t>AMS3456</t>
+  </si>
+  <si>
     <t>AMS3458</t>
   </si>
   <si>
@@ -259,24 +403,36 @@
     <t>AMS3539</t>
   </si>
   <si>
+    <t>AMS3545</t>
+  </si>
+  <si>
     <t>AMS3547</t>
   </si>
   <si>
     <t>AMS3550</t>
   </si>
   <si>
+    <t>AMS3556</t>
+  </si>
+  <si>
     <t>AMS3558</t>
   </si>
   <si>
     <t>AMS3561</t>
   </si>
   <si>
+    <t>AMS3567</t>
+  </si>
+  <si>
     <t>AMS3569</t>
   </si>
   <si>
     <t>AMS3572</t>
   </si>
   <si>
+    <t>AMS3578</t>
+  </si>
+  <si>
     <t>AMS3579</t>
   </si>
   <si>
@@ -286,6 +442,9 @@
     <t>AMS3585</t>
   </si>
   <si>
+    <t>AMS3589</t>
+  </si>
+  <si>
     <t>AMS3593</t>
   </si>
   <si>
@@ -295,6 +454,9 @@
     <t>AMS3598</t>
   </si>
   <si>
+    <t>AMS3600</t>
+  </si>
+  <si>
     <t>AMS3602</t>
   </si>
   <si>
@@ -307,21 +469,33 @@
     <t>AMS3610</t>
   </si>
   <si>
+    <t>AMS3611</t>
+  </si>
+  <si>
     <t>AMS3618</t>
   </si>
   <si>
+    <t>AMS3622</t>
+  </si>
+  <si>
     <t>AMS3624</t>
   </si>
   <si>
     <t>AMS3629</t>
   </si>
   <si>
+    <t>AMS3633</t>
+  </si>
+  <si>
     <t>AMS3723</t>
   </si>
   <si>
     <t>AMS3725</t>
   </si>
   <si>
+    <t>AMS3726</t>
+  </si>
+  <si>
     <t>AMS3727</t>
   </si>
   <si>
@@ -331,9 +505,21 @@
     <t>AMS3729</t>
   </si>
   <si>
+    <t>AMS3744</t>
+  </si>
+  <si>
+    <t>AMS3745</t>
+  </si>
+  <si>
     <t>AMS3749</t>
   </si>
   <si>
+    <t>AMS3753</t>
+  </si>
+  <si>
+    <t>AMS3756</t>
+  </si>
+  <si>
     <t>AMS3759</t>
   </si>
   <si>
@@ -400,6 +586,9 @@
     <t>AMS3834</t>
   </si>
   <si>
+    <t>AMS3847</t>
+  </si>
+  <si>
     <t>AMS3848</t>
   </si>
   <si>
@@ -415,6 +604,9 @@
     <t>AMS3853</t>
   </si>
   <si>
+    <t>AMS3854</t>
+  </si>
+  <si>
     <t>AMS3855</t>
   </si>
   <si>
@@ -427,12 +619,21 @@
     <t>AMS3859</t>
   </si>
   <si>
+    <t>AMS3860</t>
+  </si>
+  <si>
     <t>AMS3861</t>
   </si>
   <si>
+    <t>AMS3866</t>
+  </si>
+  <si>
     <t>AMS3867</t>
   </si>
   <si>
+    <t>AMS3868</t>
+  </si>
+  <si>
     <t>AMS3876</t>
   </si>
   <si>
@@ -442,9 +643,30 @@
     <t>AMS3878</t>
   </si>
   <si>
+    <t>AMS3882</t>
+  </si>
+  <si>
+    <t>AMS3883</t>
+  </si>
+  <si>
+    <t>AMS3884</t>
+  </si>
+  <si>
     <t>AMS3890</t>
   </si>
   <si>
+    <t>AMS3892</t>
+  </si>
+  <si>
+    <t>AMS3897</t>
+  </si>
+  <si>
+    <t>AMS3898</t>
+  </si>
+  <si>
+    <t>AMS3899</t>
+  </si>
+  <si>
     <t>AMS3911</t>
   </si>
   <si>
@@ -463,6 +685,27 @@
     <t>AMS3925</t>
   </si>
   <si>
+    <t>AMS3929</t>
+  </si>
+  <si>
+    <t>AMS3930</t>
+  </si>
+  <si>
+    <t>AMS3931</t>
+  </si>
+  <si>
+    <t>AMS3939</t>
+  </si>
+  <si>
+    <t>AMS3944</t>
+  </si>
+  <si>
+    <t>AMS3945</t>
+  </si>
+  <si>
+    <t>AMS3946</t>
+  </si>
+  <si>
     <t>AMS3956</t>
   </si>
   <si>
@@ -481,24 +724,81 @@
     <t>AMS3993</t>
   </si>
   <si>
+    <t>AMS3994</t>
+  </si>
+  <si>
+    <t>AMS3995</t>
+  </si>
+  <si>
+    <t># Inq w/in 3 M</t>
+  </si>
+  <si>
+    <t># Inq w/in 12 M</t>
+  </si>
+  <si>
+    <t># Inq w/in 24 M</t>
+  </si>
+  <si>
+    <t># Non-Util Inq w/in 1 Month</t>
+  </si>
+  <si>
+    <t># Non-Util Inq w/in 3 M</t>
+  </si>
+  <si>
+    <t># Non-Util Inq w/in 12 M</t>
+  </si>
+  <si>
+    <t># Non-Util Inq w/in 24 M</t>
+  </si>
+  <si>
     <t>% Inq w/in 1 Month to Inq w/in 12 M</t>
   </si>
   <si>
+    <t>% Inq w/in 1 Month to Inq w/in 24 M</t>
+  </si>
+  <si>
     <t>% Util Inq w/in 3 M to Inq w/in 12 M</t>
   </si>
   <si>
+    <t>% Util Inq w/in 3 M to Inq w/in 24 M</t>
+  </si>
+  <si>
+    <t>% Util Inq w/in 12 M to Inq w/in 24 M</t>
+  </si>
+  <si>
     <t>% Util Inq w/in 1 Month to Inq w/in 12 M</t>
   </si>
   <si>
+    <t>% Util Inq w/in 1 Month to Inq w/in 24 M</t>
+  </si>
+  <si>
     <t>% Non-Util Inq w/in 3 M to Inq w/in 12 M</t>
   </si>
   <si>
+    <t>% Non-Util Inq w/in 3 M to Inq w/in 24 M</t>
+  </si>
+  <si>
+    <t>% Non-Util Inq w/in 12 M to Inq w/in 24 M</t>
+  </si>
+  <si>
     <t>% Non-Util Inq w/in 1 Month to Inq w/in 12 M</t>
   </si>
   <si>
+    <t>% Non-Util Inq w/in 1 Month to Inq w/in 24 M</t>
+  </si>
+  <si>
+    <t># Inq w/in 6 M</t>
+  </si>
+  <si>
     <t># Util Inq w/in 6 M</t>
   </si>
   <si>
+    <t># Non-Util Inq w/in 6 M</t>
+  </si>
+  <si>
+    <t># Inq w/in 1 Month</t>
+  </si>
+  <si>
     <t># Util Inq w/in 1 Month</t>
   </si>
   <si>
@@ -514,12 +814,18 @@
     <t>Age Oldest Mortgage Trade</t>
   </si>
   <si>
+    <t>Age Oldest Retail Trade</t>
+  </si>
+  <si>
     <t>Age Newest Auto Trade</t>
   </si>
   <si>
     <t>Age Newest Dept Store Trades</t>
   </si>
   <si>
+    <t>Age Newest Retail Trade</t>
+  </si>
+  <si>
     <t>Age Newest Sales Finance Trade</t>
   </si>
   <si>
@@ -538,18 +844,30 @@
     <t># Open PerFin and StuLoan Trades</t>
   </si>
   <si>
+    <t># Open Retail Trades</t>
+  </si>
+  <si>
     <t># Open Sales Finance Trades</t>
   </si>
   <si>
+    <t xml:space="preserve"># Bkcrd Trades w/Update w/in 3 M w/ Bal &gt; $0 </t>
+  </si>
+  <si>
     <t xml:space="preserve"># Dept Store Trades w/Update w/in 3 M w/ Bal &gt; $0 </t>
   </si>
   <si>
+    <t xml:space="preserve"># Inst Trades w/Update w/in 3 M w/ Bal &gt; $0 </t>
+  </si>
+  <si>
     <t xml:space="preserve"># Retail Trades w/Update w/in 3 M w/ Bal &gt; $0 </t>
   </si>
   <si>
     <t>T Bal Open Auto Trades w/Update w/in 3 M</t>
   </si>
   <si>
+    <t>T Bal Open Bkcrd Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
     <t>T Bal Open Credit Union Trades w/Update w/in 3 M</t>
   </si>
   <si>
@@ -607,6 +925,9 @@
     <t>T Loan Amount Open Auto Trades w/Update w/in 3 M</t>
   </si>
   <si>
+    <t>T High Credit Open Bkcrd Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
     <t>T High Credit Open Dept Store Trades w/Update w/in 3 M</t>
   </si>
   <si>
@@ -622,57 +943,117 @@
     <t>T High Credit Open Retail Trades w/Update w/in 3 M</t>
   </si>
   <si>
+    <t># Retail Trades w/ PD &gt; $0</t>
+  </si>
+  <si>
+    <t>T PD  Bkcrd Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
+    <t>T PD Inst Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
     <t>T PD Retail Trades w/Update w/in 3 M</t>
   </si>
   <si>
+    <t xml:space="preserve">T PD Retail Trades </t>
+  </si>
+  <si>
     <t># 30 DPD Occur w/in 24 M Dept Store Trades</t>
   </si>
   <si>
+    <t># 30 DPD Occur w/in 24 M Retail Trades</t>
+  </si>
+  <si>
+    <t># 60 DPD Occur w/in 12 M Retail Trades</t>
+  </si>
+  <si>
     <t># 60 DPD Occur w/in 24 M Dept Store Trades</t>
   </si>
   <si>
+    <t># 60 DPD Occur w/in 24 M Retail Trades</t>
+  </si>
+  <si>
     <t># 90 DPD Occur w/in 24 M Dept Store Trades</t>
   </si>
   <si>
+    <t># 90 DPD Occur w/in 24 M Retail Trades</t>
+  </si>
+  <si>
     <t># 120-180 or More DPD Occur w/in 24 M Dept Store Trades</t>
   </si>
   <si>
+    <t># 120-180 or More DPD Occur w/in 24 M Retail Trades</t>
+  </si>
+  <si>
     <t># Dept Store Trades Satis w/in 3 M</t>
   </si>
   <si>
+    <t># Retail Trades Satis w/in 3 M</t>
+  </si>
+  <si>
+    <t># Retail Trades Satis w/in 6 M</t>
+  </si>
+  <si>
     <t># 60-180 or More DPD Occur w/in 24 M Dept Store Trades</t>
   </si>
   <si>
+    <t># 60-180 or More DPD Occur w/in 24 M Retail Trades</t>
+  </si>
+  <si>
     <t># 90-180 or More DPD Occur w/in 24 M Dept Store Trades</t>
   </si>
   <si>
+    <t># 90-180 or More DPD Occur w/in 24 M Retail Trades</t>
+  </si>
+  <si>
     <t># 60-180 or More DPD Occur w/in 12 M Dept Store Trades</t>
   </si>
   <si>
+    <t># 60-180 or More DPD Occur w/in 12 M Retail Trades</t>
+  </si>
+  <si>
     <t># 90-180 or More DPD Occur w/in 12 M Dept Store Trades</t>
   </si>
   <si>
+    <t># 90-180 or More DPD Occur w/in 12 M Retail Trades</t>
+  </si>
+  <si>
+    <t># Retail Trades Always Satis</t>
+  </si>
+  <si>
     <t># Dept Store Tr Wo Rat 30 DPD w/in 3 M</t>
   </si>
   <si>
+    <t># Retail Tr Wo Rat 30 DPD w/in 3 M</t>
+  </si>
+  <si>
     <t># Sales Finance Tr Wo Rat 30 DPD w/in 3 M</t>
   </si>
   <si>
     <t># Dept Store Tr Wo Rat 60 DPD w/in 3 M</t>
   </si>
   <si>
+    <t># Retail Tr Wo Rat 60 DPD w/in 3 M</t>
+  </si>
+  <si>
     <t># Sales Finance Tr Wo Rat 60 DPD w/in 3 M</t>
   </si>
   <si>
     <t># Dept Store Tr Wo Rat 90 DPD w/in 3 M</t>
   </si>
   <si>
+    <t># Retail Tr Wo Rat 90 DPD w/in 3 M</t>
+  </si>
+  <si>
     <t># Sales Finance Tr Wo Rat 90 DPD w/in 3 M</t>
   </si>
   <si>
     <t># Dept Store Tr Wo Rat 120-180 or More DPD w/in 3 M</t>
   </si>
   <si>
+    <t># Retail Tr Wo Rat 120-180 or More DPD w/in 3 M</t>
+  </si>
+  <si>
     <t># Sales Finance Tr Wo Rat 120-180 or More DPD w/in 3 M</t>
   </si>
   <si>
@@ -682,6 +1063,9 @@
     <t># PerFin and StuLoan Tr Wo Rat 30 DPD w/in 6 M</t>
   </si>
   <si>
+    <t># Retail Tr Wo Rat 30 DPD w/in 6 M</t>
+  </si>
+  <si>
     <t># Sales Finance Tr Wo Rat 30 DPD w/in 6 M</t>
   </si>
   <si>
@@ -691,6 +1075,9 @@
     <t># PerFin and StuLoan Tr Wo Rat 60 DPD w/in 6 M</t>
   </si>
   <si>
+    <t># Retail Tr Wo Rat 60 DPD w/in 6 M</t>
+  </si>
+  <si>
     <t># Sales Finance Tr Wo Rat 60 DPD w/in 6 M</t>
   </si>
   <si>
@@ -700,6 +1087,9 @@
     <t># PerFin and StuLoan Tr Wo Rat 90 DPD w/in 6 M</t>
   </si>
   <si>
+    <t># Retail Tr Wo Rat 90 DPD w/in 6 M</t>
+  </si>
+  <si>
     <t># Sales Finance Tr Wo Rat 90 DPD w/in 6 M</t>
   </si>
   <si>
@@ -709,6 +1099,9 @@
     <t># PerFin and StuLoan Tr Wo Rat 120-180 or More DPD w/in 6 M</t>
   </si>
   <si>
+    <t># Retail Tr Wo Rat 120-180 or More DPD w/in 6 M</t>
+  </si>
+  <si>
     <t># Sales Finance Tr Wo Rat 120-180 or More DPD w/in 6 M</t>
   </si>
   <si>
@@ -718,24 +1111,36 @@
     <t># Dept Store Tr Wo Rat Ever 30 DPD</t>
   </si>
   <si>
+    <t># Retail Tr Wo Rat Ever 30 DPD</t>
+  </si>
+  <si>
     <t># Auto Tr Wo Rat Ever 60 DPD</t>
   </si>
   <si>
     <t># Dept Store Tr Wo Rat Ever 60 DPD</t>
   </si>
   <si>
+    <t># Retail Tr Wo Rat Ever 60 DPD</t>
+  </si>
+  <si>
     <t># Auto Tr Wo Rat Ever 90 DPD</t>
   </si>
   <si>
     <t># Dept Store Tr Wo Rat Ever 90 DPD</t>
   </si>
   <si>
+    <t># Retail Tr Wo Rat Ever 90 DPD</t>
+  </si>
+  <si>
     <t># Auto Tr Wo Rat Ever 120-180 or More DPD</t>
   </si>
   <si>
     <t># Dept Store Tr Wo Rat Ever 120-180 or More DPD</t>
   </si>
   <si>
+    <t># Retail Tr Wo Rat Ever120-180 or More DPD</t>
+  </si>
+  <si>
     <t>Worst Rating w/in 3 M Auto Trades</t>
   </si>
   <si>
@@ -745,6 +1150,9 @@
     <t># Dept Store Trades w/ MajDerog Reported w/in 6 M</t>
   </si>
   <si>
+    <t># Retail Trades w/ MajDerog Reported w/in 6 M</t>
+  </si>
+  <si>
     <t># Auto Trades w/ MajDerog Event w/in 24 M</t>
   </si>
   <si>
@@ -754,6 +1162,9 @@
     <t># Mortgage Trades w/ MajDerog Event w/in 24 M</t>
   </si>
   <si>
+    <t># Retail Trades w/ MajDerog Event w/in 24 M</t>
+  </si>
+  <si>
     <t># Sales Finance Trades w/ MajDerog Event w/in 24 M</t>
   </si>
   <si>
@@ -766,21 +1177,33 @@
     <t># Mortgage Trades MajDerog</t>
   </si>
   <si>
+    <t># Retail Trades MajDerog</t>
+  </si>
+  <si>
     <t># Dept Store Trades w/ Unpaid MajDerog Event w/in 24 M</t>
   </si>
   <si>
+    <t># Retail Trades w/ Unpaid MajDerog Event w/in 24 M</t>
+  </si>
+  <si>
     <t># Sales Finance Trades w/ Unpaid MajDerog Event w/in 24 M</t>
   </si>
   <si>
     <t xml:space="preserve"># Dept Store Trades Unpaid MajDerog </t>
   </si>
   <si>
+    <t xml:space="preserve"># Retail Trades Unpaid MajDerog </t>
+  </si>
+  <si>
     <t># Open Retail Trades w/ Update w/in 3 M w/ Bal &gt;= 50% High Credit</t>
   </si>
   <si>
     <t xml:space="preserve"># Open Auto Trades w/ Update w/in 3 M w/ Bal &gt;= 75% Loan Amount </t>
   </si>
   <si>
+    <t xml:space="preserve"># Open Bkcrd Trades w/ Update w/in 3 M w/ Bal &gt;= 75% High Credit </t>
+  </si>
+  <si>
     <t xml:space="preserve"># Open Dept Store Trades w/ Update w/in 3 M w/ Bal &gt;= 75% High Credit </t>
   </si>
   <si>
@@ -790,9 +1213,21 @@
     <t xml:space="preserve"># Open Mortgage Trades w/ Update w/in 3 M w/ Bal &gt;= 75% Loan Amount </t>
   </si>
   <si>
+    <t># Retail Trades Reported w/in 3 M</t>
+  </si>
+  <si>
+    <t># Retail Trades Reported w/in 6 M</t>
+  </si>
+  <si>
     <t># Dept Store Trades Reported w/in 3 M</t>
   </si>
   <si>
+    <t># Bkcrd Trades Reported w/in 6 M</t>
+  </si>
+  <si>
+    <t>Age Newest Date Last Activity Bkcrd Trades Paid as Agreed</t>
+  </si>
+  <si>
     <t>Age Newest Date Last Activity Trades Other Than Paid as Agreed</t>
   </si>
   <si>
@@ -859,6 +1294,9 @@
     <t>% Open Dept Store Trades to Dept Store Trades</t>
   </si>
   <si>
+    <t>T Bal Bkcrd Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
     <t>T Bal Credit Union Trades w/Update w/in 3 M</t>
   </si>
   <si>
@@ -874,6 +1312,9 @@
     <t>T Bal Sales Finance Trades w/Update w/in 3 M</t>
   </si>
   <si>
+    <t>% Bal to High Credit Open Bkcrd Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
     <t>% Bal to High Credit Open Dept Store Trades w/Update w/in 3 M</t>
   </si>
   <si>
@@ -886,12 +1327,21 @@
     <t>% Bal to T Loan Amount Open Mortgage Trades w/Update w/in 3 M</t>
   </si>
   <si>
+    <t>% T PD to T Bal Bkcrd Trades w/Update w/in 3 M</t>
+  </si>
+  <si>
     <t>% T PD to T Bal Retail Trades w/Update w/in 3 M</t>
   </si>
   <si>
+    <t>% Bkcrd Trades Satis w/in 3 M to Bkcrd Trades Reported w/in 3 M</t>
+  </si>
+  <si>
     <t>% Dept Store Trades Satis w/in 3 M to Dept Store Trades Reported w/in 3 M</t>
   </si>
   <si>
+    <t>% Inst Trades Satis w/in 3 M to Inst Trades Reported w/in 3 M</t>
+  </si>
+  <si>
     <t># Dept Store Tr Wo Rat 60 DPD or Worse w/in 3 M or MajDerog Event w/in 24 M</t>
   </si>
   <si>
@@ -901,9 +1351,30 @@
     <t># Dept Store Tr Wo Rat 120-180 or More DPD or Worse w/in 3 M or MajDerog Event w/in 24 M</t>
   </si>
   <si>
+    <t># Retail Tr Wo Rat 60 DPD or Worse w/in 3 M or MajDerog Event w/in 24 M</t>
+  </si>
+  <si>
+    <t># Retail Tr Wo Rat 90 DPD or Worse w/in 3 M or MajDerog Event w/in 24 M</t>
+  </si>
+  <si>
+    <t># Retail Tr Wo Rat 120-180 or More DPD or Worse w/in 3 M or MajDerog Event w/in 24 M</t>
+  </si>
+  <si>
     <t># Dept Store Tr Wo Rat No Worse Than 59 DPD w/in 3 M</t>
   </si>
   <si>
+    <t># Retail Tr Wo Rat No Worse Than 59 DPD w/in 3 M</t>
+  </si>
+  <si>
+    <t>% Bkcrd Tr Wo Rat 60 DPD or Worse w/in 3 M or MajDerog Event w/in 24 M to Bkcrd Trades Reported w/in 3 M</t>
+  </si>
+  <si>
+    <t>% Bkcrd Tr Wo Rat 90 DPD or Worse w/in 3 M or MajDerog Event w/in 24 M to Bkcrd Trades Reported w/in 3 M</t>
+  </si>
+  <si>
+    <t>% Bkcrd Tr Wo Rat 120-180 or More DPD or Worse w/in 3 M or MajDerog Event w/in 24 M to Bkcrd Trades Reported w/in 3 M</t>
+  </si>
+  <si>
     <t>T Collection Amount 3rd Party Collections w/in 12 M</t>
   </si>
   <si>
@@ -922,6 +1393,27 @@
     <t># Dept Store Tr Wo Rat 120-180 or More DPD or Worse w/in 6 M or MajDerog Event w/in 24 M</t>
   </si>
   <si>
+    <t># Retail Tr Wo Rat 60 DPD or Worse w/in 6 M or MajDerog Event w/in 24 M</t>
+  </si>
+  <si>
+    <t># Retail Tr Wo Rat 90 DPD or Worse w/in 6 M or MajDerog Event w/in 24 M</t>
+  </si>
+  <si>
+    <t># Retail Tr Wo Rat 120-180 or More DPD or Worse w/in 6 M or MajDerog Event w/in 24 M</t>
+  </si>
+  <si>
+    <t>% Bkcrd Trades Satis w/in 6 M to Bkcrd Trades Reported w/in 6 M</t>
+  </si>
+  <si>
+    <t>% Bkcrd Tr Wo Rat 60 DPD or Worse w/in 6 M or MajDerog Event w/in 24 M to Bkcrd Trades Reported w/in 6 M</t>
+  </si>
+  <si>
+    <t>% Bkcrd Tr Wo Rat 90 DPD or Worse w/in 6 M or MajDerog Event w/in 24 M to Bkcrd Trades Reported w/in 6 M</t>
+  </si>
+  <si>
+    <t>% Bkcrd Tr Wo Rat 120-180 or More DPD or Worse w/in 6 M or MajDerog Event w/in 24 M to Bkcrd Trades Reported w/in 6 M</t>
+  </si>
+  <si>
     <t xml:space="preserve"># Dept Store Tr Wo Rat Ever 60 DPD or Worse </t>
   </si>
   <si>
@@ -938,6 +1430,12 @@
   </si>
   <si>
     <t>% Inq w/in 3 M to Inq w/in 12 M</t>
+  </si>
+  <si>
+    <t>% Inq w/in 3 M to Inq w/in 24 M</t>
+  </si>
+  <si>
+    <t>% Inq w/in 12 M to Inq w/in 24 M</t>
   </si>
 </sst>
 </file>
@@ -1295,7 +1793,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B154"/>
+  <dimension ref="A1:B237"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1314,7 +1812,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1322,7 +1820,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1330,7 +1828,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1338,7 +1836,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>158</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1346,7 +1844,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>159</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1354,7 +1852,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1362,7 +1860,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>161</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1370,7 +1868,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>162</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1378,7 +1876,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1386,7 +1884,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>164</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1394,7 +1892,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>165</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1402,7 +1900,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>166</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1410,7 +1908,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>167</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1418,7 +1916,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>168</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1426,7 +1924,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>169</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1434,7 +1932,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>170</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1442,7 +1940,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>171</v>
+        <v>254</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1450,7 +1948,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>172</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1458,7 +1956,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>173</v>
+        <v>256</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1466,7 +1964,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>174</v>
+        <v>257</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1474,7 +1972,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>175</v>
+        <v>258</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1482,7 +1980,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>176</v>
+        <v>259</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1490,7 +1988,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>177</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1498,7 +1996,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>178</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1506,7 +2004,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>179</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1514,7 +2012,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>180</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1522,7 +2020,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>181</v>
+        <v>264</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1530,7 +2028,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>182</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1538,7 +2036,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>183</v>
+        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1546,7 +2044,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>184</v>
+        <v>267</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1554,7 +2052,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>185</v>
+        <v>268</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1562,7 +2060,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>186</v>
+        <v>269</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1570,7 +2068,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>187</v>
+        <v>270</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1578,7 +2076,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>188</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1586,7 +2084,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>189</v>
+        <v>272</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1594,7 +2092,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>190</v>
+        <v>273</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1602,7 +2100,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>191</v>
+        <v>274</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1610,7 +2108,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>192</v>
+        <v>275</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1618,7 +2116,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>193</v>
+        <v>276</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1626,7 +2124,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>194</v>
+        <v>277</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1634,7 +2132,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>195</v>
+        <v>278</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1642,7 +2140,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>196</v>
+        <v>279</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1650,7 +2148,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>197</v>
+        <v>280</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1658,7 +2156,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>198</v>
+        <v>281</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1666,7 +2164,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>199</v>
+        <v>282</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1674,7 +2172,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>200</v>
+        <v>283</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1682,7 +2180,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>201</v>
+        <v>284</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1690,7 +2188,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>202</v>
+        <v>285</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1698,7 +2196,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>203</v>
+        <v>286</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1706,7 +2204,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>204</v>
+        <v>287</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1714,7 +2212,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>205</v>
+        <v>288</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1722,7 +2220,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>206</v>
+        <v>289</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1730,7 +2228,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>207</v>
+        <v>290</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1738,7 +2236,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>208</v>
+        <v>291</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1746,7 +2244,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>209</v>
+        <v>292</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1754,7 +2252,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>210</v>
+        <v>293</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1762,7 +2260,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>211</v>
+        <v>294</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1770,7 +2268,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>212</v>
+        <v>295</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1778,7 +2276,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>213</v>
+        <v>296</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1786,7 +2284,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>214</v>
+        <v>297</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1794,7 +2292,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>215</v>
+        <v>298</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1802,7 +2300,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>216</v>
+        <v>299</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1810,7 +2308,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>217</v>
+        <v>300</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1818,7 +2316,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>218</v>
+        <v>301</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1826,7 +2324,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>219</v>
+        <v>302</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1834,7 +2332,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>220</v>
+        <v>303</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1842,7 +2340,7 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>221</v>
+        <v>304</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1850,7 +2348,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>222</v>
+        <v>305</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1858,7 +2356,7 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>223</v>
+        <v>306</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1866,7 +2364,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>224</v>
+        <v>307</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1874,7 +2372,7 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>225</v>
+        <v>308</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1882,7 +2380,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>226</v>
+        <v>309</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1890,7 +2388,7 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>227</v>
+        <v>310</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1898,7 +2396,7 @@
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>228</v>
+        <v>311</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1906,7 +2404,7 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>229</v>
+        <v>312</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1914,7 +2412,7 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>230</v>
+        <v>313</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1922,7 +2420,7 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>231</v>
+        <v>314</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1930,7 +2428,7 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>232</v>
+        <v>315</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1938,7 +2436,7 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>233</v>
+        <v>316</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1946,7 +2444,7 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>234</v>
+        <v>317</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1954,7 +2452,7 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>235</v>
+        <v>318</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1962,7 +2460,7 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>236</v>
+        <v>319</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1970,7 +2468,7 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>237</v>
+        <v>320</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1978,7 +2476,7 @@
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>238</v>
+        <v>321</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1986,7 +2484,7 @@
         <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>239</v>
+        <v>322</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1994,7 +2492,7 @@
         <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>240</v>
+        <v>323</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -2002,7 +2500,7 @@
         <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>241</v>
+        <v>324</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -2010,7 +2508,7 @@
         <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>242</v>
+        <v>325</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -2018,7 +2516,7 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>243</v>
+        <v>326</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -2026,7 +2524,7 @@
         <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>244</v>
+        <v>327</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -2034,7 +2532,7 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>245</v>
+        <v>328</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -2042,7 +2540,7 @@
         <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>246</v>
+        <v>329</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -2050,7 +2548,7 @@
         <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>247</v>
+        <v>330</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -2058,7 +2556,7 @@
         <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>248</v>
+        <v>331</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -2066,7 +2564,7 @@
         <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>249</v>
+        <v>332</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -2074,7 +2572,7 @@
         <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>250</v>
+        <v>333</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -2082,7 +2580,7 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>251</v>
+        <v>334</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -2090,7 +2588,7 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>252</v>
+        <v>335</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -2098,7 +2596,7 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>253</v>
+        <v>336</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -2106,7 +2604,7 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>254</v>
+        <v>337</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -2114,7 +2612,7 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>255</v>
+        <v>338</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -2122,7 +2620,7 @@
         <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>256</v>
+        <v>339</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -2130,7 +2628,7 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>257</v>
+        <v>340</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2138,7 +2636,7 @@
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>258</v>
+        <v>341</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -2146,7 +2644,7 @@
         <v>106</v>
       </c>
       <c r="B106" t="s">
-        <v>259</v>
+        <v>342</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2154,7 +2652,7 @@
         <v>107</v>
       </c>
       <c r="B107" t="s">
-        <v>260</v>
+        <v>343</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2162,7 +2660,7 @@
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>261</v>
+        <v>344</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -2170,7 +2668,7 @@
         <v>109</v>
       </c>
       <c r="B109" t="s">
-        <v>262</v>
+        <v>345</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -2178,7 +2676,7 @@
         <v>110</v>
       </c>
       <c r="B110" t="s">
-        <v>263</v>
+        <v>346</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -2186,7 +2684,7 @@
         <v>111</v>
       </c>
       <c r="B111" t="s">
-        <v>264</v>
+        <v>347</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -2194,7 +2692,7 @@
         <v>112</v>
       </c>
       <c r="B112" t="s">
-        <v>265</v>
+        <v>348</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2202,7 +2700,7 @@
         <v>113</v>
       </c>
       <c r="B113" t="s">
-        <v>266</v>
+        <v>349</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2210,7 +2708,7 @@
         <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>267</v>
+        <v>350</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2218,7 +2716,7 @@
         <v>115</v>
       </c>
       <c r="B115" t="s">
-        <v>268</v>
+        <v>351</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2226,7 +2724,7 @@
         <v>116</v>
       </c>
       <c r="B116" t="s">
-        <v>269</v>
+        <v>352</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2234,7 +2732,7 @@
         <v>117</v>
       </c>
       <c r="B117" t="s">
-        <v>270</v>
+        <v>353</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -2242,7 +2740,7 @@
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>271</v>
+        <v>354</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2250,7 +2748,7 @@
         <v>119</v>
       </c>
       <c r="B119" t="s">
-        <v>272</v>
+        <v>355</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2258,7 +2756,7 @@
         <v>120</v>
       </c>
       <c r="B120" t="s">
-        <v>273</v>
+        <v>356</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2266,7 +2764,7 @@
         <v>121</v>
       </c>
       <c r="B121" t="s">
-        <v>274</v>
+        <v>357</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2274,7 +2772,7 @@
         <v>122</v>
       </c>
       <c r="B122" t="s">
-        <v>275</v>
+        <v>358</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2282,7 +2780,7 @@
         <v>123</v>
       </c>
       <c r="B123" t="s">
-        <v>276</v>
+        <v>359</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2290,7 +2788,7 @@
         <v>124</v>
       </c>
       <c r="B124" t="s">
-        <v>277</v>
+        <v>360</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2298,7 +2796,7 @@
         <v>125</v>
       </c>
       <c r="B125" t="s">
-        <v>278</v>
+        <v>361</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -2306,7 +2804,7 @@
         <v>126</v>
       </c>
       <c r="B126" t="s">
-        <v>279</v>
+        <v>362</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2314,7 +2812,7 @@
         <v>127</v>
       </c>
       <c r="B127" t="s">
-        <v>280</v>
+        <v>363</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2322,7 +2820,7 @@
         <v>128</v>
       </c>
       <c r="B128" t="s">
-        <v>281</v>
+        <v>364</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2330,7 +2828,7 @@
         <v>129</v>
       </c>
       <c r="B129" t="s">
-        <v>282</v>
+        <v>365</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2338,7 +2836,7 @@
         <v>130</v>
       </c>
       <c r="B130" t="s">
-        <v>283</v>
+        <v>366</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2346,7 +2844,7 @@
         <v>131</v>
       </c>
       <c r="B131" t="s">
-        <v>284</v>
+        <v>367</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -2354,7 +2852,7 @@
         <v>132</v>
       </c>
       <c r="B132" t="s">
-        <v>285</v>
+        <v>368</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -2362,7 +2860,7 @@
         <v>133</v>
       </c>
       <c r="B133" t="s">
-        <v>286</v>
+        <v>369</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2370,7 +2868,7 @@
         <v>134</v>
       </c>
       <c r="B134" t="s">
-        <v>287</v>
+        <v>370</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2378,7 +2876,7 @@
         <v>135</v>
       </c>
       <c r="B135" t="s">
-        <v>288</v>
+        <v>371</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2386,7 +2884,7 @@
         <v>136</v>
       </c>
       <c r="B136" t="s">
-        <v>289</v>
+        <v>372</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2394,7 +2892,7 @@
         <v>137</v>
       </c>
       <c r="B137" t="s">
-        <v>290</v>
+        <v>373</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2402,7 +2900,7 @@
         <v>138</v>
       </c>
       <c r="B138" t="s">
-        <v>291</v>
+        <v>374</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2410,7 +2908,7 @@
         <v>139</v>
       </c>
       <c r="B139" t="s">
-        <v>292</v>
+        <v>375</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2418,7 +2916,7 @@
         <v>140</v>
       </c>
       <c r="B140" t="s">
-        <v>293</v>
+        <v>376</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2426,7 +2924,7 @@
         <v>141</v>
       </c>
       <c r="B141" t="s">
-        <v>294</v>
+        <v>377</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2434,7 +2932,7 @@
         <v>142</v>
       </c>
       <c r="B142" t="s">
-        <v>295</v>
+        <v>378</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2442,7 +2940,7 @@
         <v>143</v>
       </c>
       <c r="B143" t="s">
-        <v>296</v>
+        <v>379</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2450,7 +2948,7 @@
         <v>144</v>
       </c>
       <c r="B144" t="s">
-        <v>297</v>
+        <v>380</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2458,7 +2956,7 @@
         <v>145</v>
       </c>
       <c r="B145" t="s">
-        <v>298</v>
+        <v>381</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2466,7 +2964,7 @@
         <v>146</v>
       </c>
       <c r="B146" t="s">
-        <v>299</v>
+        <v>382</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2474,7 +2972,7 @@
         <v>147</v>
       </c>
       <c r="B147" t="s">
-        <v>300</v>
+        <v>383</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2482,7 +2980,7 @@
         <v>148</v>
       </c>
       <c r="B148" t="s">
-        <v>301</v>
+        <v>384</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2490,7 +2988,7 @@
         <v>149</v>
       </c>
       <c r="B149" t="s">
-        <v>302</v>
+        <v>385</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2498,7 +2996,7 @@
         <v>150</v>
       </c>
       <c r="B150" t="s">
-        <v>303</v>
+        <v>386</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2506,7 +3004,7 @@
         <v>151</v>
       </c>
       <c r="B151" t="s">
-        <v>304</v>
+        <v>387</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2514,7 +3012,7 @@
         <v>152</v>
       </c>
       <c r="B152" t="s">
-        <v>305</v>
+        <v>388</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -2522,7 +3020,7 @@
         <v>153</v>
       </c>
       <c r="B153" t="s">
-        <v>306</v>
+        <v>389</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -2530,7 +3028,671 @@
         <v>154</v>
       </c>
       <c r="B154" t="s">
-        <v>307</v>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" t="s">
+        <v>155</v>
+      </c>
+      <c r="B155" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" t="s">
+        <v>156</v>
+      </c>
+      <c r="B156" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>157</v>
+      </c>
+      <c r="B157" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" t="s">
+        <v>158</v>
+      </c>
+      <c r="B158" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" t="s">
+        <v>159</v>
+      </c>
+      <c r="B159" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" t="s">
+        <v>160</v>
+      </c>
+      <c r="B160" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" t="s">
+        <v>161</v>
+      </c>
+      <c r="B161" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" t="s">
+        <v>162</v>
+      </c>
+      <c r="B162" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" t="s">
+        <v>163</v>
+      </c>
+      <c r="B163" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" t="s">
+        <v>164</v>
+      </c>
+      <c r="B164" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165" t="s">
+        <v>165</v>
+      </c>
+      <c r="B165" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166" t="s">
+        <v>166</v>
+      </c>
+      <c r="B166" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167" t="s">
+        <v>167</v>
+      </c>
+      <c r="B167" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168" t="s">
+        <v>168</v>
+      </c>
+      <c r="B168" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169" t="s">
+        <v>169</v>
+      </c>
+      <c r="B169" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170" t="s">
+        <v>170</v>
+      </c>
+      <c r="B170" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171" t="s">
+        <v>171</v>
+      </c>
+      <c r="B171" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172" t="s">
+        <v>172</v>
+      </c>
+      <c r="B172" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173" t="s">
+        <v>173</v>
+      </c>
+      <c r="B173" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" t="s">
+        <v>174</v>
+      </c>
+      <c r="B174" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="A175" t="s">
+        <v>175</v>
+      </c>
+      <c r="B175" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176" t="s">
+        <v>176</v>
+      </c>
+      <c r="B176" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" t="s">
+        <v>177</v>
+      </c>
+      <c r="B177" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" t="s">
+        <v>178</v>
+      </c>
+      <c r="B178" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" t="s">
+        <v>179</v>
+      </c>
+      <c r="B179" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180" t="s">
+        <v>180</v>
+      </c>
+      <c r="B180" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181" t="s">
+        <v>181</v>
+      </c>
+      <c r="B181" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182" t="s">
+        <v>182</v>
+      </c>
+      <c r="B182" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183" t="s">
+        <v>183</v>
+      </c>
+      <c r="B183" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="A184" t="s">
+        <v>184</v>
+      </c>
+      <c r="B184" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185" t="s">
+        <v>185</v>
+      </c>
+      <c r="B185" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186" t="s">
+        <v>186</v>
+      </c>
+      <c r="B186" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
+      <c r="A187" t="s">
+        <v>187</v>
+      </c>
+      <c r="B187" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188" t="s">
+        <v>188</v>
+      </c>
+      <c r="B188" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
+      <c r="A189" t="s">
+        <v>189</v>
+      </c>
+      <c r="B189" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="A190" t="s">
+        <v>190</v>
+      </c>
+      <c r="B190" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
+      <c r="A191" t="s">
+        <v>191</v>
+      </c>
+      <c r="B191" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
+      <c r="A192" t="s">
+        <v>192</v>
+      </c>
+      <c r="B192" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
+      <c r="A193" t="s">
+        <v>193</v>
+      </c>
+      <c r="B193" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194" t="s">
+        <v>194</v>
+      </c>
+      <c r="B194" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
+      <c r="A195" t="s">
+        <v>195</v>
+      </c>
+      <c r="B195" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196" t="s">
+        <v>196</v>
+      </c>
+      <c r="B196" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
+      <c r="A197" t="s">
+        <v>197</v>
+      </c>
+      <c r="B197" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2">
+      <c r="A198" t="s">
+        <v>198</v>
+      </c>
+      <c r="B198" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2">
+      <c r="A199" t="s">
+        <v>199</v>
+      </c>
+      <c r="B199" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2">
+      <c r="A200" t="s">
+        <v>200</v>
+      </c>
+      <c r="B200" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2">
+      <c r="A201" t="s">
+        <v>201</v>
+      </c>
+      <c r="B201" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2">
+      <c r="A202" t="s">
+        <v>202</v>
+      </c>
+      <c r="B202" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2">
+      <c r="A203" t="s">
+        <v>203</v>
+      </c>
+      <c r="B203" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2">
+      <c r="A204" t="s">
+        <v>204</v>
+      </c>
+      <c r="B204" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2">
+      <c r="A205" t="s">
+        <v>205</v>
+      </c>
+      <c r="B205" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2">
+      <c r="A206" t="s">
+        <v>206</v>
+      </c>
+      <c r="B206" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2">
+      <c r="A207" t="s">
+        <v>207</v>
+      </c>
+      <c r="B207" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2">
+      <c r="A208" t="s">
+        <v>208</v>
+      </c>
+      <c r="B208" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2">
+      <c r="A209" t="s">
+        <v>209</v>
+      </c>
+      <c r="B209" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2">
+      <c r="A210" t="s">
+        <v>210</v>
+      </c>
+      <c r="B210" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2">
+      <c r="A211" t="s">
+        <v>211</v>
+      </c>
+      <c r="B211" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2">
+      <c r="A212" t="s">
+        <v>212</v>
+      </c>
+      <c r="B212" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2">
+      <c r="A213" t="s">
+        <v>213</v>
+      </c>
+      <c r="B213" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="A214" t="s">
+        <v>214</v>
+      </c>
+      <c r="B214" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2">
+      <c r="A215" t="s">
+        <v>215</v>
+      </c>
+      <c r="B215" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2">
+      <c r="A216" t="s">
+        <v>216</v>
+      </c>
+      <c r="B216" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2">
+      <c r="A217" t="s">
+        <v>217</v>
+      </c>
+      <c r="B217" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2">
+      <c r="A218" t="s">
+        <v>218</v>
+      </c>
+      <c r="B218" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2">
+      <c r="A219" t="s">
+        <v>219</v>
+      </c>
+      <c r="B219" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2">
+      <c r="A220" t="s">
+        <v>220</v>
+      </c>
+      <c r="B220" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2">
+      <c r="A221" t="s">
+        <v>221</v>
+      </c>
+      <c r="B221" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2">
+      <c r="A222" t="s">
+        <v>222</v>
+      </c>
+      <c r="B222" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2">
+      <c r="A223" t="s">
+        <v>223</v>
+      </c>
+      <c r="B223" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
+      <c r="A224" t="s">
+        <v>224</v>
+      </c>
+      <c r="B224" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2">
+      <c r="A225" t="s">
+        <v>225</v>
+      </c>
+      <c r="B225" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2">
+      <c r="A226" t="s">
+        <v>226</v>
+      </c>
+      <c r="B226" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2">
+      <c r="A227" t="s">
+        <v>227</v>
+      </c>
+      <c r="B227" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2">
+      <c r="A228" t="s">
+        <v>228</v>
+      </c>
+      <c r="B228" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2">
+      <c r="A229" t="s">
+        <v>229</v>
+      </c>
+      <c r="B229" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2">
+      <c r="A230" t="s">
+        <v>230</v>
+      </c>
+      <c r="B230" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2">
+      <c r="A231" t="s">
+        <v>231</v>
+      </c>
+      <c r="B231" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2">
+      <c r="A232" t="s">
+        <v>232</v>
+      </c>
+      <c r="B232" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2">
+      <c r="A233" t="s">
+        <v>233</v>
+      </c>
+      <c r="B233" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2">
+      <c r="A234" t="s">
+        <v>234</v>
+      </c>
+      <c r="B234" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2">
+      <c r="A235" t="s">
+        <v>235</v>
+      </c>
+      <c r="B235" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2">
+      <c r="A236" t="s">
+        <v>236</v>
+      </c>
+      <c r="B236" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2">
+      <c r="A237" t="s">
+        <v>237</v>
+      </c>
+      <c r="B237" t="s">
+        <v>473</v>
       </c>
     </row>
   </sheetData>

</xml_diff>